<commit_message>
Fixed the Android v1.7.8 App BLE curtain piaring in tick #193
</commit_message>
<xml_diff>
--- a/App_Release/Android/v1.7.8/Zeus_Android_v1_7_8.xlsx
+++ b/App_Release/Android/v1.7.8/Zeus_Android_v1_7_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\summe\Documents\000-Github\RYSE_Testing_record\App_Release\Android\v1.7.8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC1D3D6-C8C1-4195-9191-AEEDD64842AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE4B11C-939D-4CC7-BF67-2D528C5723DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="381">
   <si>
     <t>Code</t>
   </si>
@@ -1071,9 +1071,6 @@
   </si>
   <si>
     <t>22-07-2025</t>
-  </si>
-  <si>
-    <t>Submitted bug report</t>
   </si>
   <si>
     <t>Android_App_Test_Suite_v1.7.8_Shade_Part5_22July2025</t>
@@ -1359,7 +1356,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1525,7 +1522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1562,8 +1559,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1612,7 +1608,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4366,8 +4362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA5EB23-85E7-4EC6-9FFB-9E2F32772CB4}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4380,15 +4376,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="15" t="s">
         <v>375</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="15" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
@@ -4419,7 +4415,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>317</v>
@@ -4543,13 +4539,13 @@
         <v>92</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>317</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -4582,7 +4578,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>317</v>
@@ -4679,7 +4675,7 @@
         <v>321</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -4807,7 +4803,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>317</v>
@@ -4878,7 +4874,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>317</v>
@@ -4897,13 +4893,13 @@
         <v>318</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -4921,7 +4917,7 @@
         <v>324</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -4941,7 +4937,7 @@
         <v>323</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -4961,7 +4957,7 @@
         <v>326</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -4999,7 +4995,7 @@
         <v>326</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -5016,7 +5012,7 @@
         <v>317</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F39" s="25"/>
     </row>
@@ -5028,16 +5024,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>343</v>
-      </c>
       <c r="F40" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -5048,13 +5044,13 @@
         <v>47</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F41" s="25" t="s">
         <v>327</v>
@@ -5092,7 +5088,7 @@
         <v>317</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F43" s="25"/>
     </row>
@@ -5107,13 +5103,13 @@
         <v>330</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5125,7 +5121,7 @@
         <v>107</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>317</v>
@@ -5150,7 +5146,7 @@
         <v>329</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5179,16 +5175,16 @@
         <v>117</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5208,7 +5204,7 @@
         <v>329</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5246,7 +5242,7 @@
         <v>329</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5266,7 +5262,7 @@
         <v>329</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5277,16 +5273,16 @@
         <v>133</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E54" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5297,16 +5293,16 @@
         <v>134</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E55" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="F55" s="17" t="s">
         <v>347</v>
-      </c>
-      <c r="F55" s="17" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5335,13 +5331,13 @@
         <v>116</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F57" s="17"/>
     </row>
@@ -5353,13 +5349,13 @@
         <v>117</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F58" s="6"/>
     </row>
@@ -5381,7 +5377,7 @@
         <v>13</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>317</v>
@@ -5403,7 +5399,7 @@
         <v>317</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -5419,7 +5415,7 @@
         <v>317</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F63" s="25"/>
     </row>
@@ -5431,13 +5427,13 @@
         <v>50</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F64" s="6"/>
     </row>
@@ -5455,7 +5451,7 @@
         <v>317</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F65" s="1"/>
     </row>
@@ -5473,7 +5469,7 @@
         <v>317</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F66" s="25"/>
     </row>
@@ -5485,16 +5481,16 @@
         <v>53</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -5506,7 +5502,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>317</v>
@@ -5522,13 +5518,13 @@
         <v>104</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>317</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F70" s="1"/>
     </row>
@@ -5538,13 +5534,13 @@
         <v>102</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>317</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F71" s="25"/>
     </row>
@@ -5556,13 +5552,13 @@
         <v>76</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F72" s="17"/>
     </row>
@@ -5586,13 +5582,13 @@
         <v>78</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F74" s="17"/>
     </row>
@@ -5604,13 +5600,13 @@
         <v>141</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>317</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F75" s="25"/>
     </row>
@@ -5622,13 +5618,13 @@
         <v>142</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D76" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F76" s="17"/>
     </row>
@@ -5637,19 +5633,19 @@
         <v>139</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>317</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -5660,13 +5656,13 @@
         <v>144</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>317</v>
       </c>
       <c r="E78" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F78" s="20"/>
     </row>
@@ -5686,7 +5682,7 @@
         <v>15</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D80" s="31" t="s">
         <v>317</v>
@@ -5702,13 +5698,13 @@
         <v>73</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>317</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F81" s="1"/>
     </row>
@@ -5720,16 +5716,16 @@
         <v>74</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E82" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -5740,13 +5736,13 @@
         <v>75</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D83" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F83" s="1"/>
     </row>
@@ -5759,7 +5755,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>317</v>
@@ -5775,13 +5771,13 @@
         <v>68</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D86" s="17" t="s">
         <v>317</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F86" s="1"/>
     </row>
@@ -5793,13 +5789,13 @@
         <v>69</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>317</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F87" s="6"/>
     </row>
@@ -5807,61 +5803,61 @@
       <c r="A89" t="s">
         <v>105</v>
       </c>
-      <c r="B89" s="36" t="s">
-        <v>334</v>
+      <c r="B89" s="53" t="s">
+        <v>333</v>
       </c>
       <c r="F89" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="F90" s="36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B91" s="53" t="s">
         <v>335</v>
       </c>
-      <c r="F90" s="54" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="36" t="s">
-        <v>336</v>
-      </c>
       <c r="F91" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B92" s="37" t="s">
-        <v>377</v>
+      <c r="B92" s="53" t="s">
+        <v>376</v>
       </c>
       <c r="F92" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="53" t="s">
+        <v>379</v>
+      </c>
+      <c r="F93" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B94" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="F93" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>381</v>
-      </c>
       <c r="F94" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -5924,7 +5920,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D102:D1048576 D1:D96">
+  <conditionalFormatting sqref="D1:D96 D102:D1048576">
     <cfRule type="cellIs" dxfId="133" priority="1" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
@@ -5989,17 +5985,17 @@
         <v>15</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -6224,17 +6220,17 @@
         <v>16</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -6410,12 +6406,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -7497,16 +7493,16 @@
         <v>9</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7825,19 +7821,19 @@
         <v>10</v>
       </c>
       <c r="C1" s="30"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8137,19 +8133,19 @@
       <c r="C10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -8161,17 +8157,17 @@
       <c r="C11" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="46"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -8329,13 +8325,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8523,24 +8519,24 @@
         <v>12</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="52"/>
     </row>
     <row r="2" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -9174,24 +9170,24 @@
         <v>107</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="52"/>
     </row>
     <row r="2" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -9867,20 +9863,20 @@
         <v>13</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="52"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10270,29 +10266,29 @@
         <v>14</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="52"/>
     </row>
     <row r="2" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">

</xml_diff>